<commit_message>
Iniciada implementação motor de similaridade entre entidades do grafo
</commit_message>
<xml_diff>
--- a/_data/powerbi/fioce_prodpubl_2017_2024.xlsx
+++ b/_data/powerbi/fioce_prodpubl_2017_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,10 +523,8 @@
       <c r="J2" t="n">
         <v>5330</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Alice Paula Di Sabatino Guimarães</t>
-        </is>
+      <c r="K2" t="n">
+        <v>14.89</v>
       </c>
     </row>
     <row r="3">
@@ -562,10 +560,8 @@
       <c r="J3" t="n">
         <v>2750</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Ana Cláudia de Araújo Teixeira</t>
-        </is>
+      <c r="K3" t="n">
+        <v>14.29</v>
       </c>
     </row>
     <row r="4">
@@ -601,10 +597,8 @@
       <c r="J4" t="n">
         <v>2600</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Ana Camila Oliveira Alves</t>
-        </is>
+      <c r="K4" t="n">
+        <v>5.26</v>
       </c>
     </row>
     <row r="5">
@@ -640,10 +634,8 @@
       <c r="J5" t="n">
         <v>2595</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Adriana Costa Bacelo</t>
-        </is>
+      <c r="K5" t="n">
+        <v>14.58</v>
       </c>
     </row>
     <row r="6">
@@ -679,10 +671,8 @@
       <c r="J6" t="n">
         <v>2120</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Anna Carolina Machado Marinho</t>
-        </is>
+      <c r="K6" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -718,10 +708,8 @@
       <c r="J7" t="n">
         <v>1775</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Anya Pimentel Gomes Fernandes Vieira Meyer</t>
-        </is>
+      <c r="K7" t="n">
+        <v>15.15</v>
       </c>
     </row>
     <row r="8">
@@ -757,10 +745,8 @@
       <c r="J8" t="n">
         <v>1640</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Carla Freire Celedonio Fernandes</t>
-        </is>
+      <c r="K8" t="n">
+        <v>5.88</v>
       </c>
     </row>
     <row r="9">
@@ -796,10 +782,8 @@
       <c r="J9" t="n">
         <v>1525</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Claudia Stutz Zubieta</t>
-        </is>
+      <c r="K9" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="10">
@@ -835,10 +819,8 @@
       <c r="J10" t="n">
         <v>1490</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Clarissa Romero Teixeira</t>
-        </is>
+      <c r="K10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -874,10 +856,8 @@
       <c r="J11" t="n">
         <v>1415</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Dayane Alves Costa</t>
-        </is>
+      <c r="K11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -913,10 +893,8 @@
       <c r="J12" t="n">
         <v>1325</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Donat Alexander de Chapeaurouge</t>
-        </is>
+      <c r="K12" t="n">
+        <v>3.7</v>
       </c>
     </row>
     <row r="13">
@@ -952,10 +930,8 @@
       <c r="J13" t="n">
         <v>1190</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Eduardo Ruback dos Santos</t>
-        </is>
+      <c r="K13" t="n">
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -991,10 +967,8 @@
       <c r="J14" t="n">
         <v>1155</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Fabio Miyajima</t>
-        </is>
+      <c r="K14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1030,10 +1004,8 @@
       <c r="J15" t="n">
         <v>1135</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Fernando Braga Stehling Dias</t>
-        </is>
+      <c r="K15" t="n">
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="16">
@@ -1069,10 +1041,8 @@
       <c r="J16" t="n">
         <v>1000</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Fernando Ferreira Carneiro</t>
-        </is>
+      <c r="K16" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -1108,10 +1078,8 @@
       <c r="J17" t="n">
         <v>960</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Galba Freire Moita</t>
-        </is>
+      <c r="K17" t="n">
+        <v>9.09</v>
       </c>
     </row>
     <row r="18">
@@ -1147,10 +1115,8 @@
       <c r="J18" t="n">
         <v>920</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
-        </is>
+      <c r="K18" t="n">
+        <v>14.29</v>
       </c>
     </row>
     <row r="19">
@@ -1186,172 +1152,162 @@
       <c r="J19" t="n">
         <v>740</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Gilvan Pessoa Furtado</t>
-        </is>
+      <c r="K19" t="n">
+        <v>22.22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Maximiliano Ponte</t>
+          <t>Ana Carolina Matias Dinelly Pinto</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>270</v>
+        <v>105</v>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E20" t="n">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="F20" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="H20" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J20" t="n">
-        <v>680</v>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Ivana Cristina de Holanda Cunha Barreto</t>
-        </is>
+        <v>730</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Vanira Matos Pessoa</t>
+          <t>Maximiliano Ponte</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>150</v>
+        <v>270</v>
       </c>
       <c r="C21" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="E21" t="n">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="F21" t="n">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="G21" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>675</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Jaime Ribeiro Filho</t>
-        </is>
+        <v>680</v>
+      </c>
+      <c r="K21" t="n">
+        <v>5.26</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Marcela Helena Gambim Fonseca</t>
+          <t>Vanira Matos Pessoa</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C22" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D22" t="n">
+        <v>40</v>
+      </c>
+      <c r="E22" t="n">
         <v>20</v>
       </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
       <c r="F22" t="n">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="G22" t="n">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="H22" t="n">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="I22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>640</v>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>João Hermínio Martins da Silva</t>
-        </is>
+        <v>675</v>
+      </c>
+      <c r="K22" t="n">
+        <v>11.11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Regis Bernardo Brandim Gomes</t>
+          <t>Marcela Helena Gambim Fonseca</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E23" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="G23" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="H23" t="n">
         <v>180</v>
       </c>
       <c r="I23" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="J23" t="n">
-        <v>600</v>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>José Luís Passos Cordeiro</t>
-        </is>
+        <v>640</v>
+      </c>
+      <c r="K23" t="n">
+        <v>14.29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Ruback dos Santos</t>
+          <t>Regis Bernardo Brandim Gomes</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1364,40 +1320,38 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G24" t="n">
-        <v>270</v>
+        <v>160</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="I24" t="n">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="J24" t="n">
-        <v>360</v>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Luiz Odorico Monteiro de Andrade</t>
-        </is>
+        <v>600</v>
+      </c>
+      <c r="K24" t="n">
+        <v>9.09</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Anna Carolina Machado Marinho</t>
+          <t>Clarissa Perdigao Mello Ferraz</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="C25" t="n">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -1406,127 +1360,121 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="I25" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="J25" t="n">
-        <v>330</v>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>Marcela Helena Gambim Fonseca</t>
-        </is>
+        <v>590</v>
+      </c>
+      <c r="K25" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Marlos de Medeiros Chaves</t>
+          <t>Eduardo Ruback dos Santos</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J26" t="n">
-        <v>300</v>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Marcos Roberto Lourenzoni</t>
-        </is>
+        <v>360</v>
+      </c>
+      <c r="K26" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Adriana Costa Bacelo</t>
+          <t>Anna Carolina Machado Marinho</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D27" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="G27" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I27" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="J27" t="n">
-        <v>285</v>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>Márcio Flávio Moura de Araújo</t>
-        </is>
+        <v>330</v>
+      </c>
+      <c r="K27" t="n">
+        <v>33.33</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Venúcia Bruna Magalhães Pereira</t>
+          <t>Marlos de Medeiros Chaves</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D28" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F28" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1535,76 +1483,72 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>260</v>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Margareth Borges Coutinho Gallo</t>
-        </is>
+        <v>300</v>
+      </c>
+      <c r="K28" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Claudia Stutz Zubieta</t>
+          <t>Adriana Costa Bacelo</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G29" t="n">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="H29" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
         <v>80</v>
       </c>
       <c r="J29" t="n">
-        <v>260</v>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Marlos de Medeiros Chaves</t>
-        </is>
+        <v>285</v>
+      </c>
+      <c r="K29" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Galba Freire Moita</t>
+          <t>Júlio César Martins Ximenes</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C30" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E30" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="G30" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1613,18 +1557,16 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>185</v>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Maximiliano Ponte</t>
-        </is>
+        <v>280</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Alice Paula Di Sabatino Guimarães</t>
+          <t>Claudia Stutz Zubieta</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1640,40 +1582,38 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J31" t="n">
-        <v>170</v>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>Raphael Trevizani</t>
-        </is>
+        <v>260</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Dayane Alves Costa</t>
+          <t>Venúcia Bruna Magalhães Pereira</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1685,43 +1625,41 @@
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>150</v>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>Regis Bernardo Brandim Gomes</t>
-        </is>
+        <v>260</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Ana Camila Oliveira Alves</t>
+          <t>Galba Freire Moita</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F33" t="n">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="G33" t="n">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1730,18 +1668,16 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>120</v>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Roberto Nicolete</t>
-        </is>
+        <v>185</v>
+      </c>
+      <c r="K33" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Ana Cláudia de Araújo Teixeira</t>
+          <t>Alice Paula Di Sabatino Guimarães</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1757,34 +1693,32 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="G34" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>110</v>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Roberto Wagner Júnior Freire de Freitas</t>
-        </is>
+        <v>170</v>
+      </c>
+      <c r="K34" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Margareth Borges Coutinho Gallo</t>
+          <t>Dayane Alves Costa</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1796,34 +1730,32 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
+        <v>40</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>20</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>150</v>
+      </c>
+      <c r="K35" t="n">
         <v>100</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>100</v>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>Sharmênia de Araújo Soares Nuto</t>
-        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
+          <t>Ana Camila Oliveira Alves</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1835,34 +1767,32 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H36" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>100</v>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>Vanira Matos Pessoa</t>
-        </is>
+        <v>120</v>
+      </c>
+      <c r="K36" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Raphael Trevizani</t>
+          <t>Ana Cláudia de Araújo Teixeira</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -1877,34 +1807,32 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>90</v>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>Venúcia Bruna Magalhães Pereira</t>
-        </is>
+        <v>110</v>
+      </c>
+      <c r="K37" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Donat Alexander de Chapeaurouge</t>
+          <t>Giovanny Augusto Camacho Antevere Mazzarotto</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C38" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1913,63 +1841,207 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>80</v>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>Fernanda Savicki de Almeida</t>
-        </is>
+        <v>100</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
+          <t>Margareth Borges Coutinho Gallo</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>100</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>100</v>
+      </c>
+      <c r="K39" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Antonio Marcos Aires Barbosa</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>15</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>80</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>95</v>
+      </c>
+      <c r="K40" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Raphael Trevizani</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>90</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>90</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Donat Alexander de Chapeaurouge</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>80</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>80</v>
+      </c>
+      <c r="K42" t="n">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
           <t>Fernanda Savicki de Almeida</t>
         </is>
       </c>
-      <c r="B39" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
         <v>5</v>
       </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" t="n">
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
         <v>5</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Caroline Pereira Bittencourt Passaes</t>
-        </is>
+      <c r="K43" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>